<commit_message>
swipe job. Check in before new .data
</commit_message>
<xml_diff>
--- a/swipejob/document/SWIPEJOB - BA.xlsx
+++ b/swipejob/document/SWIPEJOB - BA.xlsx
@@ -872,19 +872,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C28" sqref="C27:H28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="11.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -992,7 +992,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="9" t="s">
         <v>93</v>
       </c>
@@ -1008,7 +1008,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1290,16 +1290,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="43.625" customWidth="1"/>
-    <col min="3" max="4" width="45.75" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
+    <col min="3" max="4" width="45.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1326,7 +1327,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="120">
+    <row r="2" spans="1:7" ht="135" hidden="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="75">
+    <row r="3" spans="1:7" ht="90" hidden="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1360,7 +1361,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="75">
+    <row r="4" spans="1:7" ht="90" hidden="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75">
+    <row r="5" spans="1:7" ht="90">
       <c r="B5" t="s">
         <v>61</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="60">
+    <row r="6" spans="1:7" ht="60" hidden="1">
       <c r="B6" t="s">
         <v>60</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60">
+    <row r="7" spans="1:7" ht="75" hidden="1">
       <c r="B7" t="s">
         <v>48</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="75">
+    <row r="8" spans="1:7" ht="75" hidden="1">
       <c r="B8" t="s">
         <v>51</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="90">
+    <row r="9" spans="1:7" ht="120" hidden="1">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" hidden="1">
       <c r="B11" t="s">
         <v>65</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="120">
+    <row r="12" spans="1:7" ht="135" hidden="1">
       <c r="B12" t="s">
         <v>67</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" hidden="1">
       <c r="B13" t="s">
         <v>70</v>
       </c>
@@ -1494,7 +1495,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75">
+    <row r="14" spans="1:7" ht="90">
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" hidden="1">
       <c r="B15" t="s">
         <v>73</v>
       </c>
@@ -1526,7 +1527,11 @@
       <c r="C17" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F15"/>
+  <autoFilter ref="A1:F15">
+    <filterColumn colId="5">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1542,10 +1547,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.125" customWidth="1"/>
-    <col min="3" max="3" width="45.75" customWidth="1"/>
-    <col min="4" max="4" width="40.25" customWidth="1"/>
-    <col min="5" max="5" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1571,7 +1576,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75">
+    <row r="2" spans="1:7" ht="90">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1606,16 +1611,16 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="38.375" customWidth="1"/>
-    <col min="3" max="3" width="41.125" customWidth="1"/>
-    <col min="4" max="4" width="45.625" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1664,7 +1669,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" ht="120">
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="135">
       <c r="B6" s="10" t="s">
         <v>81</v>
       </c>
@@ -1675,7 +1680,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="60">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="75">
       <c r="B7" s="10" t="s">
         <v>83</v>
       </c>
@@ -1686,7 +1691,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" ht="135">
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="150">
       <c r="B8" s="10" t="s">
         <v>84</v>
       </c>
@@ -1710,7 +1715,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="10" customFormat="1" ht="120">
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="135">
       <c r="B11" s="10" t="s">
         <v>86</v>
       </c>
@@ -1718,7 +1723,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="10" customFormat="1" ht="75">
+    <row r="12" spans="1:6" s="10" customFormat="1" ht="90">
       <c r="B12" s="10" t="s">
         <v>87</v>
       </c>
@@ -1731,7 +1736,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="10" customFormat="1" ht="75">
+    <row r="14" spans="1:6" s="10" customFormat="1" ht="90">
       <c r="B14" s="10" t="s">
         <v>67</v>
       </c>
@@ -1739,7 +1744,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="10" customFormat="1" ht="105">
+    <row r="15" spans="1:6" s="10" customFormat="1" ht="120">
       <c r="B15" s="10" t="s">
         <v>70</v>
       </c>
@@ -1774,7 +1779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>